<commit_message>
Editing excel file for ecurefbase test
</commit_message>
<xml_diff>
--- a/reman/tests/Base_réf_ECU_test.xlsx
+++ b/reman/tests/Base_réf_ECU_test.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
   <si>
     <t xml:space="preserve">Reference OE</t>
   </si>
@@ -143,9 +143,6 @@
     <t xml:space="preserve">REF XELON</t>
   </si>
   <si>
-    <t xml:space="preserve">9812345678</t>
-  </si>
-  <si>
     <t xml:space="preserve">ECU_TEST1</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t xml:space="preserve">ECU_TEST1_HW9812345678</t>
   </si>
   <si>
-    <t xml:space="preserve">9887654321</t>
-  </si>
-  <si>
     <t xml:space="preserve">ECU_TEST2</t>
   </si>
   <si>
@@ -170,9 +164,6 @@
     <t xml:space="preserve">ECU_TEST2_HW9887654321</t>
   </si>
   <si>
-    <t xml:space="preserve">9600000000</t>
-  </si>
-  <si>
     <t xml:space="preserve">ECU_TEST3</t>
   </si>
   <si>
@@ -180,9 +171,6 @@
   </si>
   <si>
     <t xml:space="preserve">ECU_TEST3_HW9600000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9611111111</t>
   </si>
   <si>
     <t xml:space="preserve">ECU_TEST4</t>
@@ -784,7 +772,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -827,105 +815,105 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>39</v>
+      <c r="A2" s="3" t="n">
+        <v>9812345678</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>1612345678</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>9812345678</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>9812345678</v>
       </c>
       <c r="G2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>44</v>
+      <c r="A3" s="3" t="n">
+        <v>9887654321</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>1687654321</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>9887654321</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>44</v>
+      <c r="F3" s="3" t="n">
+        <v>9887654321</v>
       </c>
       <c r="G3" s="18"/>
       <c r="H3" s="17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>48</v>
+      <c r="A4" s="3" t="n">
+        <v>9600000000</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1600000000</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>9600000000</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>9600000000</v>
       </c>
       <c r="G4" s="15" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>52</v>
+      <c r="A5" s="3" t="n">
+        <v>9611111111</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>1611111111</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>9611111111</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>9611111111</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,22 +924,22 @@
         <v>1611111111</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>9611111111</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>9622222222</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Translation update, adding update and datatable templates for Default model
</commit_message>
<xml_diff>
--- a/reman/tests/Base_réf_ECU_test.xlsx
+++ b/reman/tests/Base_réf_ECU_test.xlsx
@@ -327,7 +327,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -376,27 +376,35 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -767,7 +775,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -775,237 +783,173 @@
       <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="12" width="17.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="13.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="19.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="12" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="7.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="17.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="12" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="12" width="25.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="12" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="n">
         <v>9812345678</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="17" t="n">
         <v>1612345678</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="17" t="n">
         <v>9812345678</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="17" t="n">
         <v>9812345678</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="n">
         <v>9887654321</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="17" t="n">
         <v>1687654321</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="17" t="n">
         <v>9887654321</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="17" t="n">
         <v>9887654321</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="17" t="s">
+      <c r="G3" s="20"/>
+      <c r="H3" s="19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="n">
         <v>9600000000</v>
       </c>
-      <c r="B4" s="3" t="n">
+      <c r="B4" s="17" t="n">
         <v>1600000000</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="17" t="n">
         <v>9600000000</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="17" t="n">
         <v>9600000000</v>
       </c>
-      <c r="G4" s="15" t="n">
+      <c r="G4" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="17" t="n">
         <v>1611111111</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="17" t="n">
         <v>1611111111</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="17" t="n">
         <v>9622222222</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Editing tests for REMAN cmds
</commit_message>
<xml_diff>
--- a/reman/tests/Base_réf_ECU_test.xlsx
+++ b/reman/tests/Base_réf_ECU_test.xlsx
@@ -12,7 +12,7 @@
     <sheet name="base" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">base!$A$1:$H$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">base!$A$1:$I$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">REF FNR</t>
   </si>
   <si>
-    <t xml:space="preserve">REF XELON</t>
+    <t xml:space="preserve">REF à créer </t>
   </si>
   <si>
     <t xml:space="preserve">ECU_TEST1</t>
@@ -196,7 +196,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -232,6 +232,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -327,7 +334,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -396,6 +403,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,12 +425,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -485,7 +496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -495,13 +506,12 @@
       <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -771,19 +781,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="12" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="19.44"/>
@@ -792,8 +802,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="12" width="7.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="17.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="12" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="12" width="25.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="12" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="12" width="25.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="12" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -818,135 +828,141 @@
       <c r="G1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="14"/>
+      <c r="I1" s="17" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="n">
+      <c r="A2" s="18" t="n">
         <v>9812345678</v>
       </c>
-      <c r="B2" s="17" t="n">
+      <c r="B2" s="18" t="n">
         <v>1612345678</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="17" t="n">
+      <c r="D2" s="18" t="n">
         <v>9812345678</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="17" t="n">
+      <c r="F2" s="18" t="n">
         <v>9812345678</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="19"/>
+      <c r="I2" s="20" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="n">
+      <c r="A3" s="18" t="n">
         <v>9887654321</v>
       </c>
-      <c r="B3" s="17" t="n">
+      <c r="B3" s="18" t="n">
         <v>1687654321</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="17" t="n">
+      <c r="D3" s="18" t="n">
         <v>9887654321</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="17" t="n">
+      <c r="F3" s="18" t="n">
         <v>9887654321</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="19" t="s">
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="n">
+      <c r="A4" s="18" t="n">
         <v>9600000000</v>
       </c>
-      <c r="B4" s="17" t="n">
+      <c r="B4" s="18" t="n">
         <v>1600000000</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="17" t="n">
+      <c r="D4" s="18" t="n">
         <v>9600000000</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="17" t="n">
+      <c r="F4" s="18" t="n">
         <v>9600000000</v>
       </c>
-      <c r="G4" s="18" t="n">
+      <c r="G4" s="19" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="n">
+      <c r="A5" s="18" t="n">
         <v>9611111111</v>
       </c>
-      <c r="B5" s="17" t="n">
+      <c r="B5" s="18" t="n">
         <v>1611111111</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="17" t="n">
+      <c r="D5" s="18" t="n">
         <v>9611111111</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="17" t="n">
+      <c r="F5" s="18" t="n">
         <v>9611111111</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="19"/>
+      <c r="I5" s="20" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="n">
+      <c r="A6" s="18" t="n">
         <v>9611111111</v>
       </c>
-      <c r="B6" s="17" t="n">
+      <c r="B6" s="18" t="n">
         <v>1611111111</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="17" t="n">
+      <c r="D6" s="18" t="n">
         <v>9611111111</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="17" t="n">
+      <c r="F6" s="18" t="n">
         <v>9622222222</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="19"/>
+      <c r="I6" s="20" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removing Python 3.5 and adding Python 3.8 in the Travis config
</commit_message>
<xml_diff>
--- a/reman/tests/Base_réf_ECU_test.xlsx
+++ b/reman/tests/Base_réf_ECU_test.xlsx
@@ -196,7 +196,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -232,13 +232,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -334,7 +327,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -400,10 +393,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -506,7 +495,7 @@
       <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17"/>
@@ -790,7 +779,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -829,140 +818,140 @@
         <v>37</v>
       </c>
       <c r="H1" s="14"/>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="n">
+      <c r="A2" s="17" t="n">
         <v>9812345678</v>
       </c>
-      <c r="B2" s="18" t="n">
+      <c r="B2" s="17" t="n">
         <v>1612345678</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="18" t="n">
+      <c r="D2" s="17" t="n">
         <v>9812345678</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="18" t="n">
+      <c r="F2" s="17" t="n">
         <v>9812345678</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20" t="s">
+      <c r="H2" s="18"/>
+      <c r="I2" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="n">
+      <c r="A3" s="17" t="n">
         <v>9887654321</v>
       </c>
-      <c r="B3" s="18" t="n">
+      <c r="B3" s="17" t="n">
         <v>1687654321</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="18" t="n">
+      <c r="D3" s="17" t="n">
         <v>9887654321</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="18" t="n">
+      <c r="F3" s="17" t="n">
         <v>9887654321</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="20" t="s">
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="n">
+      <c r="A4" s="17" t="n">
         <v>9600000000</v>
       </c>
-      <c r="B4" s="18" t="n">
+      <c r="B4" s="17" t="n">
         <v>1600000000</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="18" t="n">
+      <c r="D4" s="17" t="n">
         <v>9600000000</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="18" t="n">
+      <c r="F4" s="17" t="n">
         <v>9600000000</v>
       </c>
-      <c r="G4" s="19" t="n">
+      <c r="G4" s="18" t="n">
         <v>0</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="20" t="s">
+      <c r="H4" s="18"/>
+      <c r="I4" s="19" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="n">
+      <c r="A5" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="B5" s="18" t="n">
+      <c r="B5" s="17" t="n">
         <v>1611111111</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="18" t="n">
+      <c r="D5" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="18" t="n">
+      <c r="F5" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="20" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="19" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="n">
+      <c r="A6" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="B6" s="18" t="n">
+      <c r="B6" s="17" t="n">
         <v>1611111111</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="18" t="n">
+      <c r="D6" s="17" t="n">
         <v>9611111111</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="18" t="n">
+      <c r="F6" s="17" t="n">
         <v>9622222222</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20" t="s">
+      <c r="H6" s="18"/>
+      <c r="I6" s="19" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>